<commit_message>
update working hours az
</commit_message>
<xml_diff>
--- a/doc/scrum_v02_17122015.xlsx
+++ b/doc/scrum_v02_17122015.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\Semester_5\BTX8081_Software_Engineering_and_Design\Case_Studies\CS1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="120" windowWidth="16485" windowHeight="9315" activeTab="2"/>
+    <workbookView xWindow="400" yWindow="120" windowWidth="15400" windowHeight="16260" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -18,7 +13,12 @@
     <sheet name="Tabelle1" sheetId="5" r:id="rId4"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -573,7 +573,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -608,7 +608,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -823,13 +823,13 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.25" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -837,7 +837,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -845,7 +845,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -853,7 +853,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -861,7 +861,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -869,7 +869,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -877,7 +877,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -887,6 +887,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -898,20 +903,20 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="3" customFormat="1" ht="28">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -940,7 +945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" s="1" customFormat="1" ht="28">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -970,7 +975,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="56">
       <c r="A3">
         <v>2</v>
       </c>
@@ -998,7 +1003,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="84">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1026,7 +1031,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="70">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1070,7 +1075,7 @@
       <c r="X5" s="7"/>
       <c r="Y5" s="7"/>
     </row>
-    <row r="6" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="56">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1114,7 +1119,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="7" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="56">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1160,7 +1165,7 @@
       <c r="X7" s="7"/>
       <c r="Y7" s="7"/>
     </row>
-    <row r="8" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="28">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1204,7 +1209,7 @@
       <c r="X8" s="7"/>
       <c r="Y8" s="7"/>
     </row>
-    <row r="9" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="28">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1248,7 +1253,7 @@
       <c r="X9" s="7"/>
       <c r="Y9" s="7"/>
     </row>
-    <row r="10" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="28">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1292,7 +1297,7 @@
       <c r="X10" s="7"/>
       <c r="Y10" s="7"/>
     </row>
-    <row r="11" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="28">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1336,7 +1341,7 @@
       <c r="X11" s="7"/>
       <c r="Y11" s="7"/>
     </row>
-    <row r="12" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="56">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1379,7 +1384,7 @@
       <c r="X12" s="7"/>
       <c r="Y12" s="7"/>
     </row>
-    <row r="13" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -1422,7 +1427,7 @@
       <c r="X13" s="7"/>
       <c r="Y13" s="7"/>
     </row>
-    <row r="14" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="28">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -1465,7 +1470,7 @@
       <c r="X14" s="7"/>
       <c r="Y14" s="7"/>
     </row>
-    <row r="15" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="28">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -1508,7 +1513,7 @@
       <c r="X15" s="7"/>
       <c r="Y15" s="7"/>
     </row>
-    <row r="16" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="28">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1551,7 +1556,7 @@
       <c r="X16" s="7"/>
       <c r="Y16" s="7"/>
     </row>
-    <row r="17" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="28">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1594,7 +1599,7 @@
       <c r="X17" s="7"/>
       <c r="Y17" s="7"/>
     </row>
-    <row r="18" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="28">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1637,7 +1642,7 @@
       <c r="X18" s="7"/>
       <c r="Y18" s="7"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -1673,7 +1678,7 @@
       <c r="X19" s="7"/>
       <c r="Y19" s="7"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -1711,7 +1716,7 @@
       <c r="X20" s="7"/>
       <c r="Y20" s="7"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1732,7 +1737,7 @@
       <c r="X21" s="7"/>
       <c r="Y21" s="7"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -1769,7 +1774,7 @@
       <c r="X22" s="7"/>
       <c r="Y22" s="7"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1803,7 +1808,7 @@
       <c r="X23" s="7"/>
       <c r="Y23" s="7"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1832,7 +1837,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1840,27 +1850,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" customWidth="1"/>
-    <col min="3" max="3" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
-    <col min="10" max="16" width="9.140625" customWidth="1"/>
-    <col min="17" max="17" width="7.28515625" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" customWidth="1"/>
+    <col min="10" max="16" width="9.1640625" customWidth="1"/>
+    <col min="17" max="17" width="7.33203125" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="4" customFormat="1" ht="42">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1916,7 +1926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -1933,7 +1943,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21">
       <c r="A3">
         <v>1.2</v>
       </c>
@@ -1950,7 +1960,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21">
       <c r="A4">
         <v>1.3</v>
       </c>
@@ -1967,7 +1977,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21">
       <c r="A5">
         <v>1.4</v>
       </c>
@@ -1987,7 +1997,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21">
       <c r="A6">
         <v>2.1</v>
       </c>
@@ -2029,7 +2039,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21">
       <c r="A7">
         <v>2.2000000000000002</v>
       </c>
@@ -2071,7 +2081,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="A8">
         <v>2.2999999999999998</v>
       </c>
@@ -2110,7 +2120,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="A9">
         <v>2.4</v>
       </c>
@@ -2152,7 +2162,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10">
         <v>2.5</v>
       </c>
@@ -2188,7 +2198,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21">
       <c r="A11">
         <v>3.1</v>
       </c>
@@ -2230,7 +2240,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21">
       <c r="A12">
         <v>3.2</v>
       </c>
@@ -2272,7 +2282,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="A13">
         <v>3.3</v>
       </c>
@@ -2314,7 +2324,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21">
       <c r="A14">
         <v>3.4</v>
       </c>
@@ -2356,7 +2366,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21">
       <c r="A15">
         <v>3.5</v>
       </c>
@@ -2392,7 +2402,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21">
       <c r="A16">
         <v>4.0999999999999996</v>
       </c>
@@ -2428,7 +2438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>4.2</v>
       </c>
@@ -2458,7 +2468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17">
       <c r="A18">
         <v>4.3</v>
       </c>
@@ -2488,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17">
       <c r="A19">
         <v>4.4000000000000004</v>
       </c>
@@ -2517,7 +2527,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17">
       <c r="A20">
         <v>5.0999999999999996</v>
       </c>
@@ -2550,7 +2560,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>5.2</v>
       </c>
@@ -2583,7 +2593,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17">
       <c r="A22">
         <v>5.3</v>
       </c>
@@ -2616,7 +2626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17">
       <c r="A23">
         <v>5.4</v>
       </c>
@@ -2644,12 +2654,15 @@
       <c r="M23">
         <v>3</v>
       </c>
+      <c r="O23">
+        <v>3</v>
+      </c>
       <c r="Q23">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24">
         <v>5.5</v>
       </c>
@@ -2678,7 +2691,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17">
       <c r="A25">
         <v>6.1</v>
       </c>
@@ -2705,7 +2718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17">
       <c r="A26">
         <v>6.2</v>
       </c>
@@ -2732,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17">
       <c r="A27">
         <v>6.3</v>
       </c>
@@ -2759,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17">
       <c r="A28">
         <v>6.4</v>
       </c>
@@ -2786,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17">
       <c r="A29">
         <v>6.5</v>
       </c>
@@ -2809,7 +2822,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17">
       <c r="A30">
         <v>7.1</v>
       </c>
@@ -2839,7 +2852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17">
       <c r="A31">
         <v>7.2</v>
       </c>
@@ -2869,7 +2882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17">
       <c r="A32">
         <v>7.3</v>
       </c>
@@ -2902,7 +2915,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17">
       <c r="A33">
         <v>7.4</v>
       </c>
@@ -2935,7 +2948,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17">
       <c r="A34">
         <v>7.5</v>
       </c>
@@ -2964,7 +2977,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17">
       <c r="A35">
         <v>8.1</v>
       </c>
@@ -2998,12 +3011,15 @@
       <c r="M35">
         <v>0.5</v>
       </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
       <c r="Q35">
         <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36">
         <v>8.1999999999999993</v>
       </c>
@@ -3042,7 +3058,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17">
       <c r="A37">
         <v>8.3000000000000007</v>
       </c>
@@ -3071,7 +3087,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17">
       <c r="A38">
         <v>9.1</v>
       </c>
@@ -3107,7 +3123,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17">
       <c r="A39">
         <v>9.1999999999999993</v>
       </c>
@@ -3137,7 +3153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17">
       <c r="A40">
         <v>9.3000000000000007</v>
       </c>
@@ -3166,7 +3182,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17">
       <c r="A41">
         <v>10.1</v>
       </c>
@@ -3199,7 +3215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17">
       <c r="A42">
         <v>10.199999999999999</v>
       </c>
@@ -3229,7 +3245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17">
       <c r="A43">
         <v>10.3</v>
       </c>
@@ -3258,7 +3274,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17">
       <c r="A44">
         <v>18.100000000000001</v>
       </c>
@@ -3291,7 +3307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17">
       <c r="A45">
         <v>19.100000000000001</v>
       </c>
@@ -3330,7 +3346,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17">
       <c r="A46">
         <v>20.100000000000001</v>
       </c>
@@ -3360,60 +3376,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17">
       <c r="Q47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17">
       <c r="D48" s="7"/>
       <c r="Q48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:17">
       <c r="D49" s="7"/>
       <c r="Q49">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:17">
       <c r="Q50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:17">
       <c r="D51" s="7"/>
       <c r="Q51">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:17">
       <c r="D52" s="7"/>
       <c r="Q52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:17">
       <c r="D53" s="7"/>
       <c r="Q53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:17">
       <c r="Q54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:17">
       <c r="C55" t="s">
         <v>122</v>
       </c>
@@ -3440,7 +3456,7 @@
       </c>
       <c r="O55">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>8.5</v>
       </c>
       <c r="P55">
         <f t="shared" si="1"/>
@@ -3448,83 +3464,88 @@
       </c>
       <c r="Q55">
         <f t="shared" si="1"/>
-        <v>64.2</v>
-      </c>
-    </row>
-    <row r="56" spans="3:17" x14ac:dyDescent="0.25">
+        <v>68.2</v>
+      </c>
+    </row>
+    <row r="56" spans="3:17">
       <c r="D56" s="7"/>
     </row>
-    <row r="57" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:17">
       <c r="D57" s="7"/>
     </row>
-    <row r="58" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:17">
       <c r="D58" s="7"/>
     </row>
-    <row r="59" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:17">
       <c r="D59" s="7"/>
     </row>
-    <row r="61" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:17">
       <c r="D61" s="7"/>
     </row>
-    <row r="62" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:17">
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:17">
       <c r="D63" s="7"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:4">
       <c r="D65" s="7"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:4">
       <c r="D66" s="7"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:4">
       <c r="D67" s="7"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:4">
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:4">
       <c r="D70" s="7"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:4">
       <c r="D71" s="7"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:4">
       <c r="D73" s="7"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:4">
       <c r="D74" s="7"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:4">
       <c r="D75" s="7"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4">
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4">
       <c r="D77" s="7"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4">
       <c r="D79" s="7"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:4">
       <c r="D80" s="7"/>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:4">
       <c r="D81" s="7"/>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:4">
       <c r="D83" s="7"/>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:4">
       <c r="D84" s="7"/>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:4">
       <c r="D85" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3536,12 +3557,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="B2" t="s">
         <v>79</v>
       </c>
@@ -3552,7 +3573,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="6">
         <v>42336</v>
       </c>
@@ -3566,7 +3587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>86</v>
       </c>
@@ -3577,7 +3598,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="6">
         <v>42340</v>
       </c>
@@ -3591,7 +3612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="6">
         <v>42341</v>
       </c>
@@ -3605,7 +3626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="B11">
         <f>SUM(B3,B7)</f>
         <v>14</v>
@@ -3621,6 +3642,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3632,14 +3658,14 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.5" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
@@ -3653,7 +3679,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3667,7 +3693,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3683,6 +3709,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>